<commit_message>
A new line was added
</commit_message>
<xml_diff>
--- a/Xlsx file.xlsx
+++ b/Xlsx file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enot\Desktop\SF_INT QAP 1052\Mod 9\redesigned-eureka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5904AF12-4AA1-4710-A6CC-0D2F13BD64B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06934CF4-CFA1-480E-9FC3-EC6EF75A4AC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="975" windowWidth="25335" windowHeight="14625" xr2:uid="{1B28F60A-AC70-4B8C-B007-361A87B2F1DF}"/>
   </bookViews>
@@ -378,9 +378,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3450E5-BF62-4660-916C-D5C0887C74BC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -389,6 +391,11 @@
         <v>12345</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6789</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>